<commit_message>
Ajustes en caso OrdenDeCobro vacio
</commit_message>
<xml_diff>
--- a/validacion.xlsx
+++ b/validacion.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\D\Zona de Trabajo\SQL\Recaudacion-BN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zona Trabajo\SQL\Recaudacion-BN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EE1D57-5517-401A-834B-74F641C8DCF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590AB1E9-A175-428A-8B16-6AF4DAE8E8CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D083D23-69AA-4411-88FA-927F8FD39A68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8D083D23-69AA-4411-88FA-927F8FD39A68}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Envio Cabecera" sheetId="2" r:id="rId1"/>
+    <sheet name="Envio Detalle" sheetId="3" r:id="rId2"/>
+    <sheet name="Recepcion Detalle" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="116">
   <si>
     <t>CABECERA</t>
   </si>
@@ -251,13 +251,145 @@
   </si>
   <si>
     <t>018010000000200000000452886040000001461512912021031001</t>
+  </si>
+  <si>
+    <t>REGISTRO</t>
+  </si>
+  <si>
+    <t>CAMPO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>LONGITUD</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>Número del crédito cobrado </t>
+  </si>
+  <si>
+    <t>Num. de Cuota</t>
+  </si>
+  <si>
+    <t>Número de la cuota del crédito</t>
+  </si>
+  <si>
+    <t>Situación de la recuperación</t>
+  </si>
+  <si>
+    <t>Las situaciones de desembolso son:      * 02= Pagado totalmente</t>
+  </si>
+  <si>
+    <t>* 04= Pagado parcialmente</t>
+  </si>
+  <si>
+    <t>Código de moneda</t>
+  </si>
+  <si>
+    <t>Los códigos de moneda son:                  * 1 = Soles                                             * 2 = Dólares</t>
+  </si>
+  <si>
+    <t>Nombre Cliente</t>
+  </si>
+  <si>
+    <t>Fecha de caducidad</t>
+  </si>
+  <si>
+    <t>YYYYMMDD        Ej. 20050814</t>
+  </si>
+  <si>
+    <t>Indicar de la Tasa</t>
+  </si>
+  <si>
+    <t>Los indicadores de tasa son:</t>
+  </si>
+  <si>
+    <t>* 0 = Tasa determinada</t>
+  </si>
+  <si>
+    <t>* 1 = Tasa con factores</t>
+  </si>
+  <si>
+    <t>Factor Mora</t>
+  </si>
+  <si>
+    <t>8 + 7 decimales. Ej. 000000041000000 = S/. 4.1000000</t>
+  </si>
+  <si>
+    <t>Factor Compensación</t>
+  </si>
+  <si>
+    <t>Importe Gastos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenta Cliente </t>
+  </si>
+  <si>
+    <t>Cuenta del cliente, deberá tener una cuenta para soles y otra cuenta para dólares</t>
+  </si>
+  <si>
+    <t>Número de cobro</t>
+  </si>
+  <si>
+    <t>Mora</t>
+  </si>
+  <si>
+    <t>Importe de la mora:</t>
+  </si>
+  <si>
+    <t>Compensación</t>
+  </si>
+  <si>
+    <t>Importe de la compensación:</t>
+  </si>
+  <si>
+    <t>Importe Cobrado</t>
+  </si>
+  <si>
+    <t>Agencia de cobro</t>
+  </si>
+  <si>
+    <t>Código de la agencia que se ha cobrado la recuperación</t>
+  </si>
+  <si>
+    <t>Fecha de Cobro</t>
+  </si>
+  <si>
+    <t>Fecha que se ha cobrado la recuperación:                      YYYYMMDD        Ej. 20050714</t>
+  </si>
+  <si>
+    <t>Hora de Cobro</t>
+  </si>
+  <si>
+    <t>Hora que se ha cobrado la recuperación:</t>
+  </si>
+  <si>
+    <t>HHMMSS             Ej:103005</t>
+  </si>
+  <si>
+    <t>0202001798570013021GARCIA              VALERIO             EDGAR EDUARDO221032600000000053259020210313000000000000000000000000000000000000000000000000068385520000000000000000000000000000000000000000000000000000532590000520210326163309</t>
+  </si>
+  <si>
+    <t>0202001799770010021CHUMBIMUNI          SANCHEZ             CECILIA DEL P221032600000000008674120210313000000000000000000000000000000000000000000000000068385520000000000000000000000000000000000000000000000000000086741000520210326163419</t>
+  </si>
+  <si>
+    <t>0202001801390001041VELEZ               BENDEZU             VERONICA PATR221032600000000230399620210313000000000000000000000000000000000000000000000000068385520000000000000000000000000000000000000000000000000000303996000520210326163551  &lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>0202001802300006021PERALTA             MORALES             MELCHOR      221032600000000016159020210313000000000000000000000000000000000000000000000000068385520000000000000000000000000000000000000000000000000000161590000520210326163642</t>
+  </si>
+  <si>
+    <t>0202001807460008021C Y T REPRESENTACIONES S.A.                          221032600000000010130420210313000000000000000000000000000000000000000000000000068385520000000000000000000000000000000000000000000000000000101304000520210326164010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +410,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,8 +431,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -395,11 +540,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -436,6 +609,19 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,19 +646,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,132 +999,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD714456-3746-456D-9BD2-49FD6C80E586}">
-  <dimension ref="A1:A21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067F6767-FC35-40D9-9DB9-1830F354C204}">
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +1018,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -943,7 +1035,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -958,7 +1050,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -973,7 +1065,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -988,7 +1080,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +1095,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1018,7 +1110,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1033,7 +1125,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1076,7 +1168,7 @@
       <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1105,7 +1197,7 @@
       <c r="H11" s="2">
         <v>2</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="17">
         <v>226</v>
       </c>
     </row>
@@ -1254,12 +1346,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F6C1DE-071E-4594-9E29-8D6D02F43554}">
   <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1376,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1301,7 +1393,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1316,7 +1408,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
@@ -1331,7 +1423,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1346,14 +1438,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="24">
         <v>60</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -1361,23 +1453,23 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="20"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="21"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1392,7 +1484,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1407,7 +1499,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
@@ -1422,7 +1514,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
@@ -1563,10 +1655,10 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="22"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
@@ -1620,7 +1712,7 @@
       <c r="R22" t="s">
         <v>48</v>
       </c>
-      <c r="S22" s="26" t="s">
+      <c r="S22" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1676,7 +1768,7 @@
       <c r="R23" t="s">
         <v>2</v>
       </c>
-      <c r="S23" s="26" t="s">
+      <c r="S23" s="18" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1735,7 +1827,7 @@
       <c r="R24">
         <v>15</v>
       </c>
-      <c r="S24" s="26">
+      <c r="S24" s="18">
         <v>49</v>
       </c>
     </row>
@@ -3209,4 +3301,1060 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C26335-5ED5-4616-B088-D806D0528D56}">
+  <dimension ref="A1:U38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" style="40" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="64" style="40" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="32">
+        <v>2</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="32">
+        <v>60</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="35">
+        <v>8</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="38">
+        <v>1</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="35">
+        <v>15</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="35">
+        <v>15</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="35">
+        <v>15</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="35">
+        <v>11</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+      <c r="B18" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="35">
+        <v>12</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="38">
+        <v>15</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="38">
+        <v>15</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="38">
+        <v>15</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="35">
+        <v>4</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="39"/>
+      <c r="B26" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="35">
+        <v>8</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="38">
+        <v>6</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="39"/>
+      <c r="B29" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="35">
+        <v>61</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" t="s">
+        <v>88</v>
+      </c>
+      <c r="J31" t="s">
+        <v>92</v>
+      </c>
+      <c r="K31" t="s">
+        <v>94</v>
+      </c>
+      <c r="L31" t="s">
+        <v>95</v>
+      </c>
+      <c r="M31" t="s">
+        <v>96</v>
+      </c>
+      <c r="N31" t="s">
+        <v>42</v>
+      </c>
+      <c r="O31" t="s">
+        <v>99</v>
+      </c>
+      <c r="P31" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>103</v>
+      </c>
+      <c r="R31" t="s">
+        <v>104</v>
+      </c>
+      <c r="S31" t="s">
+        <v>106</v>
+      </c>
+      <c r="T31" t="s">
+        <v>108</v>
+      </c>
+      <c r="U31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>2</v>
+      </c>
+      <c r="M32" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>2</v>
+      </c>
+      <c r="P32" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>2</v>
+      </c>
+      <c r="R32" t="s">
+        <v>17</v>
+      </c>
+      <c r="S32" t="s">
+        <v>2</v>
+      </c>
+      <c r="T32" t="s">
+        <v>2</v>
+      </c>
+      <c r="U32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>60</v>
+      </c>
+      <c r="G33">
+        <v>15</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>15</v>
+      </c>
+      <c r="K33">
+        <v>15</v>
+      </c>
+      <c r="L33">
+        <v>15</v>
+      </c>
+      <c r="M33">
+        <v>11</v>
+      </c>
+      <c r="N33">
+        <v>12</v>
+      </c>
+      <c r="O33">
+        <v>15</v>
+      </c>
+      <c r="P33">
+        <v>15</v>
+      </c>
+      <c r="Q33">
+        <v>15</v>
+      </c>
+      <c r="R33">
+        <v>4</v>
+      </c>
+      <c r="S33">
+        <v>8</v>
+      </c>
+      <c r="T33">
+        <v>6</v>
+      </c>
+      <c r="U33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" t="str">
+        <f>LEFT($A34,B$33)</f>
+        <v>020200179857</v>
+      </c>
+      <c r="C34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:C$33)),C$33)</f>
+        <v>0013</v>
+      </c>
+      <c r="D34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:D$33)),D$33)</f>
+        <v>02</v>
+      </c>
+      <c r="E34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:E$33)),E$33)</f>
+        <v>1</v>
+      </c>
+      <c r="F34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:F$33)),F$33)</f>
+        <v>GARCIA              VALERIO             EDGAR EDUARDO2210326</v>
+      </c>
+      <c r="G34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:G$33)),G$33)</f>
+        <v>000000000532590</v>
+      </c>
+      <c r="H34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:H$33)),H$33)</f>
+        <v>20210313</v>
+      </c>
+      <c r="I34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:I$33)),I$33)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:J$33)),J$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="K34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:K$33)),K$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="L34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:L$33)),L$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="M34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:M$33)),M$33)</f>
+        <v>00068385520</v>
+      </c>
+      <c r="N34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:N$33)),N$33)</f>
+        <v>000000000000</v>
+      </c>
+      <c r="O34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:O$33)),O$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="P34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:P$33)),P$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="Q34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:Q$33)),Q$33)</f>
+        <v>000000000532590</v>
+      </c>
+      <c r="R34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:R$33)),R$33)</f>
+        <v>0005</v>
+      </c>
+      <c r="S34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:S$33)),S$33)</f>
+        <v>20210326</v>
+      </c>
+      <c r="T34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:T$33)),T$33)</f>
+        <v>163309</v>
+      </c>
+      <c r="U34" t="str">
+        <f>RIGHT(LEFT($A34,SUM($B$33:U$33)),U$33)</f>
+        <v>0000000000000000000000000000000000000532590000520210326163309</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" ref="B35:B38" si="0">LEFT($A35,B$33)</f>
+        <v>020200179977</v>
+      </c>
+      <c r="C35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:C$33)),C$33)</f>
+        <v>0010</v>
+      </c>
+      <c r="D35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:D$33)),D$33)</f>
+        <v>02</v>
+      </c>
+      <c r="E35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:E$33)),E$33)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:F$33)),F$33)</f>
+        <v>CHUMBIMUNI          SANCHEZ             CECILIA DEL P2210326</v>
+      </c>
+      <c r="G35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:G$33)),G$33)</f>
+        <v>000000000086741</v>
+      </c>
+      <c r="H35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:H$33)),H$33)</f>
+        <v>20210313</v>
+      </c>
+      <c r="I35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:I$33)),I$33)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:J$33)),J$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="K35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:K$33)),K$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="L35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:L$33)),L$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="M35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:M$33)),M$33)</f>
+        <v>00068385520</v>
+      </c>
+      <c r="N35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:N$33)),N$33)</f>
+        <v>000000000000</v>
+      </c>
+      <c r="O35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:O$33)),O$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="P35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:P$33)),P$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="Q35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:Q$33)),Q$33)</f>
+        <v>000000000086741</v>
+      </c>
+      <c r="R35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:R$33)),R$33)</f>
+        <v>0005</v>
+      </c>
+      <c r="S35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:S$33)),S$33)</f>
+        <v>20210326</v>
+      </c>
+      <c r="T35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:T$33)),T$33)</f>
+        <v>163419</v>
+      </c>
+      <c r="U35" t="str">
+        <f>RIGHT(LEFT($A35,SUM($B$33:U$33)),U$33)</f>
+        <v>0000000000000000000000000000000000000086741000520210326163419</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>020200180139</v>
+      </c>
+      <c r="C36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:C$33)),C$33)</f>
+        <v>0001</v>
+      </c>
+      <c r="D36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:D$33)),D$33)</f>
+        <v>04</v>
+      </c>
+      <c r="E36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:E$33)),E$33)</f>
+        <v>1</v>
+      </c>
+      <c r="F36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:F$33)),F$33)</f>
+        <v>VELEZ               BENDEZU             VERONICA PATR2210326</v>
+      </c>
+      <c r="G36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:G$33)),G$33)</f>
+        <v>000000002303996</v>
+      </c>
+      <c r="H36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:H$33)),H$33)</f>
+        <v>20210313</v>
+      </c>
+      <c r="I36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:I$33)),I$33)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:J$33)),J$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="K36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:K$33)),K$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="L36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:L$33)),L$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="M36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:M$33)),M$33)</f>
+        <v>00068385520</v>
+      </c>
+      <c r="N36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:N$33)),N$33)</f>
+        <v>000000000000</v>
+      </c>
+      <c r="O36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:O$33)),O$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="P36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:P$33)),P$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="Q36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:Q$33)),Q$33)</f>
+        <v>000000000303996</v>
+      </c>
+      <c r="R36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:R$33)),R$33)</f>
+        <v>0005</v>
+      </c>
+      <c r="S36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:S$33)),S$33)</f>
+        <v>20210326</v>
+      </c>
+      <c r="T36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:T$33)),T$33)</f>
+        <v>163551</v>
+      </c>
+      <c r="U36" t="str">
+        <f>RIGHT(LEFT($A36,SUM($B$33:U$33)),U$33)</f>
+        <v>000000000000000000000000000303996000520210326163551  &lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>020200180230</v>
+      </c>
+      <c r="C37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:C$33)),C$33)</f>
+        <v>0006</v>
+      </c>
+      <c r="D37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:D$33)),D$33)</f>
+        <v>02</v>
+      </c>
+      <c r="E37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:E$33)),E$33)</f>
+        <v>1</v>
+      </c>
+      <c r="F37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:F$33)),F$33)</f>
+        <v>PERALTA             MORALES             MELCHOR      2210326</v>
+      </c>
+      <c r="G37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:G$33)),G$33)</f>
+        <v>000000000161590</v>
+      </c>
+      <c r="H37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:H$33)),H$33)</f>
+        <v>20210313</v>
+      </c>
+      <c r="I37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:I$33)),I$33)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:J$33)),J$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="K37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:K$33)),K$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="L37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:L$33)),L$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="M37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:M$33)),M$33)</f>
+        <v>00068385520</v>
+      </c>
+      <c r="N37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:N$33)),N$33)</f>
+        <v>000000000000</v>
+      </c>
+      <c r="O37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:O$33)),O$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="P37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:P$33)),P$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="Q37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:Q$33)),Q$33)</f>
+        <v>000000000161590</v>
+      </c>
+      <c r="R37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:R$33)),R$33)</f>
+        <v>0005</v>
+      </c>
+      <c r="S37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:S$33)),S$33)</f>
+        <v>20210326</v>
+      </c>
+      <c r="T37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:T$33)),T$33)</f>
+        <v>163642</v>
+      </c>
+      <c r="U37" t="str">
+        <f>RIGHT(LEFT($A37,SUM($B$33:U$33)),U$33)</f>
+        <v>0000000000000000000000000000000000000161590000520210326163642</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>020200180746</v>
+      </c>
+      <c r="C38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:C$33)),C$33)</f>
+        <v>0008</v>
+      </c>
+      <c r="D38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:D$33)),D$33)</f>
+        <v>02</v>
+      </c>
+      <c r="E38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:E$33)),E$33)</f>
+        <v>1</v>
+      </c>
+      <c r="F38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:F$33)),F$33)</f>
+        <v>C Y T REPRESENTACIONES S.A.                          2210326</v>
+      </c>
+      <c r="G38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:G$33)),G$33)</f>
+        <v>000000000101304</v>
+      </c>
+      <c r="H38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:H$33)),H$33)</f>
+        <v>20210313</v>
+      </c>
+      <c r="I38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:I$33)),I$33)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:J$33)),J$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="K38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:K$33)),K$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="L38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:L$33)),L$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="M38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:M$33)),M$33)</f>
+        <v>00068385520</v>
+      </c>
+      <c r="N38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:N$33)),N$33)</f>
+        <v>000000000000</v>
+      </c>
+      <c r="O38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:O$33)),O$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="P38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:P$33)),P$33)</f>
+        <v>000000000000000</v>
+      </c>
+      <c r="Q38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:Q$33)),Q$33)</f>
+        <v>000000000101304</v>
+      </c>
+      <c r="R38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:R$33)),R$33)</f>
+        <v>0005</v>
+      </c>
+      <c r="S38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:S$33)),S$33)</f>
+        <v>20210326</v>
+      </c>
+      <c r="T38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:T$33)),T$33)</f>
+        <v>164010</v>
+      </c>
+      <c r="U38" t="str">
+        <f>RIGHT(LEFT($A38,SUM($B$33:U$33)),U$33)</f>
+        <v>0000000000000000000000000000000000000101304000520210326164010</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>